<commit_message>
bug: spaces are possible when registering
</commit_message>
<xml_diff>
--- a/Documents/Release 2/Status Requirements.xlsx
+++ b/Documents/Release 2/Status Requirements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Documents\GitHub\teaching-2021.prse-exemplar-team4\Documents\Release 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF6AC82-31F5-4553-BB00-B05F4B77561D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E36F01C-CF1B-447B-9033-7AA0D399FE42}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27225" windowHeight="16440" xr2:uid="{E22DF244-96C0-422A-9C79-D5B775B1642E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="21444" windowHeight="13176" xr2:uid="{E22DF244-96C0-422A-9C79-D5B775B1642E}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -539,16 +539,16 @@
   <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="52.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -559,7 +559,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -568,7 +568,7 @@
       </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -579,7 +579,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -588,7 +588,7 @@
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -597,7 +597,7 @@
       </c>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -606,7 +606,7 @@
       </c>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
@@ -615,7 +615,7 @@
       </c>
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -624,7 +624,7 @@
       </c>
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
@@ -633,7 +633,7 @@
       </c>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>23</v>
       </c>
@@ -644,16 +644,16 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>26</v>
       </c>
@@ -662,7 +662,7 @@
       </c>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>27</v>
       </c>
@@ -673,7 +673,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>30</v>
       </c>
@@ -682,7 +682,7 @@
       </c>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>31</v>
       </c>
@@ -691,7 +691,7 @@
       </c>
       <c r="C15" s="2"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>12</v>
       </c>
@@ -700,7 +700,7 @@
       </c>
       <c r="C16" s="2"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>13</v>
       </c>
@@ -709,7 +709,7 @@
       </c>
       <c r="C17" s="2"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>14</v>
       </c>
@@ -718,7 +718,7 @@
       </c>
       <c r="C18" s="2"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>15</v>
       </c>
@@ -727,7 +727,7 @@
       </c>
       <c r="C19" s="2"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>32</v>
       </c>
@@ -736,7 +736,7 @@
       </c>
       <c r="C20" s="2"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>33</v>
       </c>
@@ -745,7 +745,7 @@
       </c>
       <c r="C21" s="2"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>34</v>
       </c>
@@ -754,7 +754,7 @@
       </c>
       <c r="C22" s="2"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>16</v>
       </c>
@@ -763,7 +763,7 @@
       </c>
       <c r="C23" s="2"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>18</v>
       </c>
@@ -772,7 +772,7 @@
       </c>
       <c r="C24" s="2"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>35</v>
       </c>
@@ -783,7 +783,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>36</v>
       </c>
@@ -794,7 +794,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>19</v>
       </c>
@@ -803,7 +803,7 @@
       </c>
       <c r="C27" s="2"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>20</v>
       </c>
@@ -812,7 +812,7 @@
       </c>
       <c r="C28" s="2"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>21</v>
       </c>
@@ -823,7 +823,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>38</v>
       </c>
@@ -832,7 +832,7 @@
       </c>
       <c r="C30" s="2"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>39</v>
       </c>
@@ -841,7 +841,7 @@
       </c>
       <c r="C31" s="2"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>40</v>
       </c>
@@ -850,7 +850,7 @@
       </c>
       <c r="C32" s="2"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>41</v>
       </c>

</xml_diff>

<commit_message>
export/import with .json extension
</commit_message>
<xml_diff>
--- a/Documents/Release 2/Status Requirements.xlsx
+++ b/Documents/Release 2/Status Requirements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Documents\GitHub\teaching-2021.prse-exemplar-team4\Documents\Release 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9833384-8619-4A24-8359-AAB211A65182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D1B868E-6FA6-4F44-A9A3-F6C9FB37A76D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="21444" windowHeight="13176" xr2:uid="{E22DF244-96C0-422A-9C79-D5B775B1642E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27225" windowHeight="16440" xr2:uid="{E22DF244-96C0-422A-9C79-D5B775B1642E}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="43">
   <si>
     <t>Create Exemplar Profile</t>
   </si>
@@ -160,6 +160,9 @@
   </si>
   <si>
     <t>Sort: Contributors by ratings of contributed exemplars</t>
+  </si>
+  <si>
+    <t>by ratings?</t>
   </si>
 </sst>
 </file>
@@ -538,17 +541,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4405E4EB-DD36-4206-88CA-B517802FEBF2}">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -559,7 +562,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -568,7 +571,7 @@
       </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -579,7 +582,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -588,7 +591,7 @@
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -597,7 +600,7 @@
       </c>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -606,7 +609,7 @@
       </c>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
@@ -615,7 +618,7 @@
       </c>
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -624,7 +627,7 @@
       </c>
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
@@ -633,7 +636,7 @@
       </c>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>23</v>
       </c>
@@ -644,7 +647,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>25</v>
       </c>
@@ -653,7 +656,7 @@
       </c>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>26</v>
       </c>
@@ -662,7 +665,7 @@
       </c>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>27</v>
       </c>
@@ -673,7 +676,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>30</v>
       </c>
@@ -682,7 +685,7 @@
       </c>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>31</v>
       </c>
@@ -691,7 +694,7 @@
       </c>
       <c r="C15" s="2"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>12</v>
       </c>
@@ -700,7 +703,7 @@
       </c>
       <c r="C16" s="2"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>13</v>
       </c>
@@ -709,7 +712,7 @@
       </c>
       <c r="C17" s="2"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>14</v>
       </c>
@@ -718,7 +721,7 @@
       </c>
       <c r="C18" s="2"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>15</v>
       </c>
@@ -727,7 +730,7 @@
       </c>
       <c r="C19" s="2"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>32</v>
       </c>
@@ -736,7 +739,7 @@
       </c>
       <c r="C20" s="2"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>33</v>
       </c>
@@ -745,7 +748,7 @@
       </c>
       <c r="C21" s="2"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>34</v>
       </c>
@@ -754,7 +757,7 @@
       </c>
       <c r="C22" s="2"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>16</v>
       </c>
@@ -763,7 +766,7 @@
       </c>
       <c r="C23" s="2"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>18</v>
       </c>
@@ -772,7 +775,7 @@
       </c>
       <c r="C24" s="2"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>35</v>
       </c>
@@ -783,7 +786,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>36</v>
       </c>
@@ -794,16 +797,16 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="C27" s="2"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>20</v>
       </c>
@@ -812,7 +815,7 @@
       </c>
       <c r="C28" s="2"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>21</v>
       </c>
@@ -823,7 +826,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>38</v>
       </c>
@@ -832,30 +835,32 @@
       </c>
       <c r="C30" s="2"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C31" s="2"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C31" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="C32" s="2"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="C33" s="2"/>
     </row>

</xml_diff>